<commit_message>
comence - order pipeline works
</commit_message>
<xml_diff>
--- a/static/data/prices.xlsx
+++ b/static/data/prices.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sale" sheetId="1" state="visible" r:id="rId1"/>
@@ -453,7 +453,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="1" sqref="A2:A17 B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.390625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -660,8 +660,8 @@
   </sheetPr>
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.390625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -703,7 +703,7 @@
     <row r="2" ht="15" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Radio</t>
+          <t>UHF</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -724,7 +724,7 @@
     <row r="3" ht="15" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Radio</t>
+          <t>UHF</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -745,7 +745,7 @@
     <row r="4" ht="15" customHeight="1" s="3">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Radio</t>
+          <t>UHF</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -766,7 +766,7 @@
     <row r="5" ht="15" customHeight="1" s="3">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>Radio</t>
+          <t>UHF</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -787,7 +787,7 @@
     <row r="6" ht="15" customHeight="1" s="3">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>Radio</t>
+          <t>UHF</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -808,7 +808,7 @@
     <row r="7" ht="15" customHeight="1" s="3">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>Radio</t>
+          <t>UHF</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -829,7 +829,7 @@
     <row r="8" ht="15" customHeight="1" s="3">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>Radio</t>
+          <t>UHF</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -850,7 +850,7 @@
     <row r="9" ht="15" customHeight="1" s="3">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>Radio</t>
+          <t>UHF</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
@@ -871,7 +871,7 @@
     <row r="10" ht="15" customHeight="1" s="3">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>Radio</t>
+          <t>UHF</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -892,7 +892,7 @@
     <row r="11" ht="15" customHeight="1" s="3">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>Radio</t>
+          <t>UHF</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
@@ -913,7 +913,7 @@
     <row r="12" ht="15" customHeight="1" s="3">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>Radio</t>
+          <t>UHF</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -934,7 +934,7 @@
     <row r="13" ht="15" customHeight="1" s="3">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>Radio</t>
+          <t>UHF</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -955,7 +955,7 @@
     <row r="14" ht="15" customHeight="1" s="3">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>Radio</t>
+          <t>UHF</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -976,7 +976,7 @@
     <row r="15" ht="15" customHeight="1" s="3">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>Radio</t>
+          <t>UHF</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -997,7 +997,7 @@
     <row r="16" ht="15" customHeight="1" s="3">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>Radio</t>
+          <t>UHF</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
@@ -1018,7 +1018,7 @@
     <row r="17" ht="15" customHeight="1" s="3">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>Radio</t>
+          <t>UHF</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -1288,7 +1288,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" ht="13.8" customHeight="1" s="3">
+    <row r="30" ht="13.5" customHeight="1" s="3">
       <c r="A30" s="2" t="inlineStr">
         <is>
           <t>Mobile</t>
@@ -1309,7 +1309,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" ht="13.8" customHeight="1" s="3">
+    <row r="31" ht="13.5" customHeight="1" s="3">
       <c r="A31" s="2" t="inlineStr">
         <is>
           <t>Mega</t>
@@ -1387,13 +1387,13 @@
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C50" activeCellId="1" sqref="A2:A17 C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="1" ht="12.8" customHeight="1" s="3">
+    <row r="1" ht="12.75" customHeight="1" s="3">
       <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Name</t>
@@ -1405,7 +1405,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="12.8" customHeight="1" s="3">
+    <row r="2" ht="12.75" customHeight="1" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>EM</t>
@@ -1417,7 +1417,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="13.8" customHeight="1" s="3">
+    <row r="3" ht="13.5" customHeight="1" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>UHF</t>
@@ -1429,7 +1429,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="13.8" customHeight="1" s="3">
+    <row r="4" ht="13.5" customHeight="1" s="3">
       <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Cases</t>
@@ -1441,7 +1441,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="12.8" customHeight="1" s="3">
+    <row r="5" ht="12.75" customHeight="1" s="3">
       <c r="A5" s="2" t="inlineStr">
         <is>
           <t>Icom</t>
@@ -1453,7 +1453,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="13.8" customHeight="1" s="3">
+    <row r="6" ht="13.5" customHeight="1" s="3">
       <c r="A6" s="2" t="inlineStr">
         <is>
           <t>Batteries</t>
@@ -1465,7 +1465,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="13.8" customHeight="1" s="3">
+    <row r="7" ht="13.5" customHeight="1" s="3">
       <c r="A7" s="2" t="inlineStr">
         <is>
           <t>EMC</t>
@@ -1477,7 +1477,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="13.8" customHeight="1" s="3">
+    <row r="8" ht="13.5" customHeight="1" s="3">
       <c r="A8" s="2" t="inlineStr">
         <is>
           <t>Headset</t>
@@ -1489,7 +1489,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="12.8" customHeight="1" s="3">
+    <row r="9" ht="12.75" customHeight="1" s="3">
       <c r="A9" s="2" t="inlineStr">
         <is>
           <t>Megaphone</t>
@@ -1501,7 +1501,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="13.8" customHeight="1" s="3">
+    <row r="10" ht="13.5" customHeight="1" s="3">
       <c r="A10" s="2" t="inlineStr">
         <is>
           <t>Parrot</t>
@@ -1513,7 +1513,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="12.8" customHeight="1" s="3">
+    <row r="11" ht="12.75" customHeight="1" s="3">
       <c r="A11" s="2" t="inlineStr">
         <is>
           <t>Repeater</t>
@@ -1525,7 +1525,7 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="12.8" customHeight="1" s="3">
+    <row r="12" ht="12.75" customHeight="1" s="3">
       <c r="A12" s="2" t="inlineStr">
         <is>
           <t>Wand</t>
@@ -1537,7 +1537,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="13.8" customHeight="1" s="3">
+    <row r="13" ht="13.5" customHeight="1" s="3">
       <c r="A13" s="2" t="inlineStr">
         <is>
           <t>Aircraft</t>
@@ -1549,7 +1549,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="13.8" customHeight="1" s="3"/>
+    <row r="14" ht="13.5" customHeight="1" s="3"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>